<commit_message>
rename and add area code
</commit_message>
<xml_diff>
--- a/Centanet_Res_Area_Code.xlsx
+++ b/Centanet_Res_Area_Code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ytsang/Desktop/Github/web-scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608EA91F-F037-F94C-B663-FD61EB505EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B452BC6E-7D94-4746-8F9C-D4096673C369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24700" yWindow="880" windowWidth="14920" windowHeight="21320" xr2:uid="{7BE73C72-CA16-DA4D-9469-44605EEF3162}"/>
+    <workbookView xWindow="17800" yWindow="880" windowWidth="21820" windowHeight="21320" xr2:uid="{7BE73C72-CA16-DA4D-9469-44605EEF3162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1597,11 +1597,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA35EF13-10EB-6946-B602-A639714A26A0}">
   <dimension ref="A1:D179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="174" workbookViewId="0">
-      <selection activeCell="D180" sqref="D180"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="174" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>